<commit_message>
Updated Exhibit Setup tests.
</commit_message>
<xml_diff>
--- a/Exhibits/Add Exhibit Contract to an Invoice/Main.rvl.xlsx
+++ b/Exhibits/Add Exhibit Contract to an Invoice/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="105">
   <si>
     <t>Flow</t>
   </si>
@@ -277,6 +277,57 @@
   </si>
   <si>
     <t>ux_CheckInvoiceTotals</t>
+  </si>
+  <si>
+    <t>DoLoadObjects</t>
+  </si>
+  <si>
+    <t>objectsFilePath</t>
+  </si>
+  <si>
+    <t>C:\UX365RegressionTest\Objects.js</t>
+  </si>
+  <si>
+    <t>Navigator</t>
+  </si>
+  <si>
+    <t>Navigate</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>G_OpenAreaList</t>
+  </si>
+  <si>
+    <t>***Test adds a new main Meeting Registration identified in the MeetingData spreadsheet.</t>
+  </si>
+  <si>
+    <t>****Value for g_testname must be defined to determine row in the spreadsheet for values and objects.</t>
+  </si>
+  <si>
+    <t>*****Test must already be in an invoice with batch selected.</t>
+  </si>
+  <si>
+    <t>***Test adds a new Exhibit Contract to an invoice.</t>
+  </si>
+  <si>
+    <t>***Test adds a new Exhibit Contract for TUXr Exhibit to an invoice.</t>
+  </si>
+  <si>
+    <t>****Test must already be in an invoice with batch selected.</t>
+  </si>
+  <si>
+    <t>Create new Exhibit Contract transaction</t>
+  </si>
+  <si>
+    <t>Validate invoice totals.</t>
+  </si>
+  <si>
+    <t>Validate invoice detail for contract is created.</t>
   </si>
 </sst>
 </file>
@@ -297,7 +348,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="214">
+  <borders count="227">
     <border>
       <left/>
       <right/>
@@ -518,11 +569,24 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -737,6 +801,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="211" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="212" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="213" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="214" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="215" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="216" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="217" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="218" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="219" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="220" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="221" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="222" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="223" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="224" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="225" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="226" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,7 +823,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H56"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5546875" customWidth="true"/>
@@ -786,48 +863,37 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="193" t="s">
-        <v>41</v>
-      </c>
+      <c r="A2" s="224"/>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="192"/>
+      <c r="A3" s="223"/>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="191"/>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
+      <c r="A4" s="222"/>
     </row>
     <row r="5">
-      <c r="A5" s="190"/>
+      <c r="A5" s="220"/>
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -835,32 +901,43 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="189"/>
+      <c r="A6" s="219" t="s">
+        <v>41</v>
+      </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>92</v>
+      </c>
+      <c r="E6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="188"/>
+      <c r="A7" s="218"/>
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -877,408 +954,388 @@
         <v>51</v>
       </c>
       <c r="G7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="217"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="216"/>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="214"/>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="221"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="193" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="192"/>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="191"/>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="190"/>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="189"/>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="188"/>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="187"/>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="18">
+      <c r="A18" s="187"/>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
         <v>54</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D18" t="s">
         <v>55</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E18" t="s">
         <v>56</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F18" t="s">
         <v>51</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="186"/>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="16"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="24"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="25"/>
-      <c r="B12" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="32"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="33"/>
-      <c r="B13" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="40"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="41"/>
-      <c r="B14" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14" s="48"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="56"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="64"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="65"/>
-      <c r="B17" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="68" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="70" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="H17" s="72"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="210"/>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" t="s">
-        <v>75</v>
-      </c>
-    </row>
     <row r="19">
-      <c r="A19" s="211"/>
+      <c r="A19" s="186"/>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s">
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="198"/>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="17"/>
+      <c r="B21" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="24"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="226"/>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="25"/>
+      <c r="B23" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="32"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="33"/>
+      <c r="B24" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="40"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="41"/>
+      <c r="B25" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" s="48"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="49"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="56"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="59"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="64"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="225"/>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="65"/>
+      <c r="B29" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E29" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F29" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="G20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="212"/>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="213"/>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="73"/>
-      <c r="B23" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="75" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="76" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="77" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="G23" s="79" t="s">
-        <v>78</v>
-      </c>
-      <c r="H23" s="80"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="199"/>
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="200"/>
-      <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="203"/>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="202"/>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="201"/>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="206"/>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" t="s">
-        <v>86</v>
-      </c>
+      <c r="G29" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" s="72"/>
     </row>
     <row r="30">
-      <c r="A30" s="205"/>
+      <c r="A30" s="210"/>
       <c r="B30" t="s">
         <v>11</v>
       </c>
@@ -1289,11 +1346,11 @@
         <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="204"/>
+      <c r="A31" s="211"/>
       <c r="B31" t="s">
         <v>11</v>
       </c>
@@ -1308,7 +1365,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="209"/>
+      <c r="A32" s="198"/>
       <c r="B32" t="s">
         <v>3</v>
       </c>
@@ -1316,7 +1373,7 @@
         <v>54</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E32" t="s">
         <v>56</v>
@@ -1325,11 +1382,11 @@
         <v>51</v>
       </c>
       <c r="G32" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="208"/>
+      <c r="A33" s="212"/>
       <c r="B33" t="s">
         <v>11</v>
       </c>
@@ -1340,11 +1397,11 @@
         <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="207"/>
+      <c r="A34" s="213"/>
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -1359,104 +1416,309 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="81"/>
-      <c r="B35" s="82"/>
-      <c r="C35" s="83"/>
-      <c r="D35" s="84"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="88"/>
+      <c r="A35" s="73"/>
+      <c r="B35" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="77" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="78" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" s="80"/>
     </row>
     <row r="36">
-      <c r="A36" s="89"/>
-      <c r="B36" s="90"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="92"/>
-      <c r="E36" s="93"/>
-      <c r="F36" s="94"/>
-      <c r="G36" s="95"/>
-      <c r="H36" s="96"/>
+      <c r="A36" s="199"/>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="97"/>
-      <c r="B37" s="98"/>
-      <c r="C37" s="99"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="101"/>
-      <c r="F37" s="102"/>
-      <c r="G37" s="103"/>
-      <c r="H37" s="104"/>
+      <c r="A37" s="200"/>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="105"/>
-      <c r="B38" s="106"/>
-      <c r="C38" s="107"/>
-      <c r="D38" s="108"/>
-      <c r="E38" s="109"/>
-      <c r="F38" s="110"/>
-      <c r="G38" s="111"/>
-      <c r="H38" s="112"/>
+      <c r="A38" s="203"/>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="113"/>
-      <c r="B39" s="114"/>
-      <c r="C39" s="115"/>
-      <c r="D39" s="116"/>
-      <c r="E39" s="117"/>
-      <c r="F39" s="118"/>
-      <c r="G39" s="119"/>
-      <c r="H39" s="120"/>
+      <c r="A39" s="202"/>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="121"/>
-      <c r="B40" s="122"/>
-      <c r="C40" s="123"/>
-      <c r="D40" s="124"/>
-      <c r="E40" s="125"/>
-      <c r="F40" s="126"/>
-      <c r="G40" s="127"/>
-      <c r="H40" s="128"/>
+      <c r="A40" s="201"/>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="129"/>
-      <c r="B41" s="130"/>
-      <c r="C41" s="131"/>
-      <c r="D41" s="132"/>
-      <c r="E41" s="133"/>
-      <c r="F41" s="134"/>
-      <c r="G41" s="135"/>
-      <c r="H41" s="136"/>
+      <c r="A41" s="206"/>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" t="s">
+        <v>51</v>
+      </c>
+      <c r="G41" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="137"/>
-      <c r="B42" s="138"/>
-      <c r="C42" s="139"/>
-      <c r="D42" s="140"/>
-      <c r="E42" s="141"/>
-      <c r="F42" s="142"/>
-      <c r="G42" s="143"/>
-      <c r="H42" s="144"/>
+      <c r="A42" s="205"/>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="145"/>
-      <c r="B43" s="146"/>
-      <c r="C43" s="147"/>
-      <c r="D43" s="148"/>
-      <c r="E43" s="149"/>
-      <c r="F43" s="150"/>
-      <c r="G43" s="151"/>
-      <c r="H43" s="152"/>
+      <c r="A43" s="204"/>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="153"/>
-      <c r="B44" s="154"/>
-      <c r="C44" s="155"/>
-      <c r="D44" s="156"/>
-      <c r="E44" s="157"/>
-      <c r="F44" s="158"/>
-      <c r="G44" s="159"/>
-      <c r="H44" s="160"/>
+      <c r="A44" s="209"/>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" t="s">
+        <v>51</v>
+      </c>
+      <c r="G44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="208"/>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="207"/>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="81"/>
+      <c r="B47" s="82"/>
+      <c r="C47" s="83"/>
+      <c r="D47" s="84"/>
+      <c r="E47" s="85"/>
+      <c r="F47" s="86"/>
+      <c r="G47" s="87"/>
+      <c r="H47" s="88"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="89"/>
+      <c r="B48" s="90"/>
+      <c r="C48" s="91"/>
+      <c r="D48" s="92"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="94"/>
+      <c r="G48" s="95"/>
+      <c r="H48" s="96"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="97"/>
+      <c r="B49" s="98"/>
+      <c r="C49" s="99"/>
+      <c r="D49" s="100"/>
+      <c r="E49" s="101"/>
+      <c r="F49" s="102"/>
+      <c r="G49" s="103"/>
+      <c r="H49" s="104"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="105"/>
+      <c r="B50" s="106"/>
+      <c r="C50" s="107"/>
+      <c r="D50" s="108"/>
+      <c r="E50" s="109"/>
+      <c r="F50" s="110"/>
+      <c r="G50" s="111"/>
+      <c r="H50" s="112"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="113"/>
+      <c r="B51" s="114"/>
+      <c r="C51" s="115"/>
+      <c r="D51" s="116"/>
+      <c r="E51" s="117"/>
+      <c r="F51" s="118"/>
+      <c r="G51" s="119"/>
+      <c r="H51" s="120"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="121"/>
+      <c r="B52" s="122"/>
+      <c r="C52" s="123"/>
+      <c r="D52" s="124"/>
+      <c r="E52" s="125"/>
+      <c r="F52" s="126"/>
+      <c r="G52" s="127"/>
+      <c r="H52" s="128"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="129"/>
+      <c r="B53" s="130"/>
+      <c r="C53" s="131"/>
+      <c r="D53" s="132"/>
+      <c r="E53" s="133"/>
+      <c r="F53" s="134"/>
+      <c r="G53" s="135"/>
+      <c r="H53" s="136"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="137"/>
+      <c r="B54" s="138"/>
+      <c r="C54" s="139"/>
+      <c r="D54" s="140"/>
+      <c r="E54" s="141"/>
+      <c r="F54" s="142"/>
+      <c r="G54" s="143"/>
+      <c r="H54" s="144"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="145"/>
+      <c r="B55" s="146"/>
+      <c r="C55" s="147"/>
+      <c r="D55" s="148"/>
+      <c r="E55" s="149"/>
+      <c r="F55" s="150"/>
+      <c r="G55" s="151"/>
+      <c r="H55" s="152"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="153"/>
+      <c r="B56" s="154"/>
+      <c r="C56" s="155"/>
+      <c r="D56" s="156"/>
+      <c r="E56" s="157"/>
+      <c r="F56" s="158"/>
+      <c r="G56" s="159"/>
+      <c r="H56" s="160"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>